<commit_message>
feat: Modal de solicitação de bens e busca de patrimônios com autocomplete
- Novo modal para criar solicitações de bens na página de listagem (padrão patrimônios)
- Autocomplete com dropdown para selecionar patrimônios disponíveis (SITUACAO = 'disponível')
- Novo endpoint API: GET /api/solicitacoes-bens/patrimonio-disponivel para busca
- Novo controller SolicitacaoBemPatrimonioController com método buscarDisponivel()
- Formulário create.blade.php adaptado para funcionar dentro do modal ou como página separada
- Store() no SolicitacaoBemController retorna JSON quando chamado via modal
- Componente Alpine.js solicitacaoBemsIndex() para gerenciar modal, loading e submit
- Proteção com x-cloak e validação de valores padrão no formulário
- Email de confirmação enviado automaticamente após criar solicitação
- Redirecionamento automático para lista após salvar (reload da página)
</commit_message>
<xml_diff>
--- a/public/templates/patrimonios_lista_template.xlsx
+++ b/public/templates/patrimonios_lista_template.xlsx
@@ -60,26 +60,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B2"/>
   <sheetData>
-    <row r="1" spans="1:1" customHeight="0">
+    <row r="1" spans="1:2" customHeight="0">
       <c r="A1" s="0" t="inlineStr">
         <is>
-          <t>NUPATRIMONIO</t>
+          <t>Nº PATRIMONIO</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
-    <row r="2" spans="1:1" customHeight="0">
-      <c r="A2" s="0" t="inlineStr">
+    <row r="2" spans="1:2" customHeight="0">
+      <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>1000001</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" spans="1:1" customHeight="0">
-      <c r="A3" s="0" t="inlineStr">
-        <is>
-          <t>1000000</t>
+          <t>&lt;- PREENCHA A COLUNA A COM OS N? PARA BUSCAR MAIS ITENS</t>
         </is>
       </c>
     </row>

</xml_diff>